<commit_message>
updated function point analysis
</commit_message>
<xml_diff>
--- a/function_point_analysis/function_point_analysis.xlsx
+++ b/function_point_analysis/function_point_analysis.xlsx
@@ -1,52 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmuell.ZIMMER_NT_S1\Desktop\Studium\Semester 3\Webengineering II\decksterous\function_point_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bened\OneDrive\Dokumente\VSCode\decksterous\function_point_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AB4169-BD4C-4765-B6BB-1235F19EA2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1153D3-E3E7-40B4-99A0-8A5E877E3D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
     <sheet name="Change Appearane" sheetId="11" r:id="rId2"/>
-    <sheet name="Create_Custom_Rules" sheetId="10" r:id="rId3"/>
-    <sheet name="Search_Lobbies" sheetId="9" r:id="rId4"/>
-    <sheet name="Trade_Items" sheetId="8" r:id="rId5"/>
-    <sheet name="Marketplace" sheetId="7" r:id="rId6"/>
-    <sheet name="Create_Lobby" sheetId="6" r:id="rId7"/>
-    <sheet name="Invite_Friends" sheetId="4" r:id="rId8"/>
-    <sheet name="Signin" sheetId="3" r:id="rId9"/>
-    <sheet name="Create_Deck" sheetId="2" r:id="rId10"/>
-    <sheet name="Signup" sheetId="5" r:id="rId11"/>
+    <sheet name="Show_Rankings" sheetId="12" r:id="rId3"/>
+    <sheet name="Buy_Shop_Item" sheetId="13" r:id="rId4"/>
+    <sheet name="Create_Custom_Rules" sheetId="10" r:id="rId5"/>
+    <sheet name="Search_Lobbies" sheetId="9" r:id="rId6"/>
+    <sheet name="Trade_Items" sheetId="8" r:id="rId7"/>
+    <sheet name="Marketplace" sheetId="7" r:id="rId8"/>
+    <sheet name="Create_Lobby" sheetId="6" r:id="rId9"/>
+    <sheet name="Invite_Friends" sheetId="4" r:id="rId10"/>
+    <sheet name="Signin" sheetId="3" r:id="rId11"/>
+    <sheet name="Create_Deck" sheetId="2" r:id="rId12"/>
+    <sheet name="Signup" sheetId="5" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>Use-Case</t>
   </si>
@@ -85,6 +76,15 @@
   </si>
   <si>
     <t>Change Appearance</t>
+  </si>
+  <si>
+    <t>Show Rankings</t>
+  </si>
+  <si>
+    <t>Buy Shop Item</t>
+  </si>
+  <si>
+    <t>Marketplace (Community)</t>
   </si>
 </sst>
 </file>
@@ -1411,6 +1411,104 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
+      <xdr:colOff>153288</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>58434</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B031834-4B8C-F771-62BC-B4DEF6784DD6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="6363588" cy="9202434"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>296167</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>144171</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7513CA09-D8B0-7B1F-A34F-F28F3F080BA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="6392167" cy="9288171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>343799</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>77513</xdr:rowOff>
@@ -1449,7 +1547,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1553,6 +1651,260 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16A66FFF-1827-5A47-3274-29A60A3628DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="3057525"/>
+          <a:ext cx="6638925" cy="8420100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B808CFD-3D09-0542-F18B-B7B9D156F0E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="7448550" cy="2876550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5116DD4F-6D34-AF6F-C232-96D8E22957C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="6524625" cy="3105150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98D02AEE-42B6-301E-E36F-7E2986E871E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="3228975"/>
+          <a:ext cx="6943725" cy="8372475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1596,7 +1948,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1645,7 +1997,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1694,7 +2046,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1743,7 +2095,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1781,104 +2133,6 @@
         <a:xfrm>
           <a:off x="0" y="182880"/>
           <a:ext cx="4778154" cy="6546147"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>153288</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>58434</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Grafik 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B031834-4B8C-F771-62BC-B4DEF6784DD6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="190500"/>
-          <a:ext cx="6363588" cy="9202434"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>296167</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>144171</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Grafik 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7513CA09-D8B0-7B1F-A34F-F28F3F080BA2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="190500"/>
-          <a:ext cx="6392167" cy="9288171"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2165,20 +2419,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2189,7 +2443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2200,7 +2454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2211,7 +2465,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2222,7 +2476,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2233,7 +2487,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2244,15 +2498,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>93.5</v>
       </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2260,7 +2517,7 @@
         <v>48.6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2268,7 +2525,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2276,12 +2533,34 @@
         <v>59.3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
         <v>13.3</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>44.9</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2294,6 +2573,51 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6857B391-FEA7-47A3-9F99-22327DDC951B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2156572D-0BD8-4313-87D6-D16985B4AD17}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O12" sqref="O11:O12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B8081F3-5AAF-4596-9C44-15EC04CA5584}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2301,9 +2625,9 @@
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2315,7 +2639,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2438DC60-D44D-4B85-99A9-3776944D865B}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2323,9 +2647,9 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2341,16 +2665,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87DA006-AF29-4661-8CD4-701B8D97AF51}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -2362,6 +2686,56 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D183B08B-6A90-4E77-928A-66056B5B2F56}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51CACB6B-307B-4E5F-9D1A-021F0E8EB085}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B8C725-F3E1-4020-8C11-61655DFB6FFA}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2369,12 +2743,12 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2386,7 +2760,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D4AE14-9D14-45DD-861D-E0E864BD92FB}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2394,12 +2768,12 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2410,7 +2784,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70794A90-7F01-49F6-BCBD-8CDE1B39DB48}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2418,9 +2792,9 @@
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -2431,7 +2805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F24B76-832B-4A5A-9E3C-68A3E05460DC}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2439,9 +2813,9 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2452,7 +2826,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29CB4DF7-B2D5-4EB0-95AE-A20052BF04E7}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2460,56 +2834,11 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6857B391-FEA7-47A3-9F99-22327DDC951B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2156572D-0BD8-4313-87D6-D16985B4AD17}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O12" sqref="O11:O12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>